<commit_message>
adc corrected, still waiting for the new LCD, please kill me
</commit_message>
<xml_diff>
--- a/Docs/1 - keyboard layout.xlsx
+++ b/Docs/1 - keyboard layout.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="30">
   <si>
     <t>∙</t>
   </si>
@@ -95,6 +95,15 @@
   </si>
   <si>
     <t>GND</t>
+  </si>
+  <si>
+    <t>→</t>
+  </si>
+  <si>
+    <t>old conn</t>
+  </si>
+  <si>
+    <t>new conn</t>
   </si>
 </sst>
 </file>
@@ -170,7 +179,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -505,11 +514,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -613,16 +631,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -643,9 +652,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -966,7 +991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -987,17 +1012,17 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
       <c r="O1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1008,25 +1033,25 @@
         <v>14</v>
       </c>
       <c r="S1" s="1"/>
-      <c r="T1" s="40">
+      <c r="T1" s="47">
         <v>6</v>
       </c>
-      <c r="U1" s="40"/>
-      <c r="V1" s="40"/>
-      <c r="W1" s="40"/>
-      <c r="X1" s="39">
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="46">
         <v>5</v>
       </c>
-      <c r="Y1" s="39"/>
-      <c r="Z1" s="39"/>
-      <c r="AA1" s="39"/>
-      <c r="AB1" s="39"/>
-      <c r="AC1" s="39"/>
-      <c r="AD1" s="39"/>
-      <c r="AE1" s="39"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="46"/>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="46"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="15">
@@ -1065,14 +1090,14 @@
       <c r="M2" s="21">
         <v>15</v>
       </c>
-      <c r="N2" s="44" t="s">
+      <c r="N2" s="41" t="s">
         <v>1</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="P2" s="1"/>
-      <c r="Q2" s="46">
+      <c r="Q2" s="43">
         <v>1</v>
       </c>
       <c r="R2" s="1" t="s">
@@ -1107,7 +1132,7 @@
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A3" s="49"/>
+      <c r="A3" s="39"/>
       <c r="B3" s="15">
         <v>0</v>
       </c>
@@ -1144,12 +1169,12 @@
       <c r="M3" s="22">
         <v>7</v>
       </c>
-      <c r="N3" s="45"/>
+      <c r="N3" s="42"/>
       <c r="O3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="P3" s="1"/>
-      <c r="Q3" s="46"/>
+      <c r="Q3" s="43"/>
       <c r="R3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1192,12 +1217,12 @@
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
       <c r="Q4" s="3"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -1215,22 +1240,22 @@
       <c r="AE4" s="1"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48" t="s">
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
       <c r="N5" s="38" t="s">
         <v>1</v>
       </c>
@@ -1239,25 +1264,25 @@
         <v>14</v>
       </c>
       <c r="S5" s="1"/>
-      <c r="T5" s="39">
+      <c r="T5" s="46">
         <v>4</v>
       </c>
-      <c r="U5" s="39"/>
-      <c r="V5" s="39"/>
-      <c r="W5" s="39"/>
-      <c r="X5" s="39"/>
-      <c r="Y5" s="39"/>
-      <c r="Z5" s="39"/>
-      <c r="AA5" s="39"/>
-      <c r="AB5" s="40">
+      <c r="U5" s="46"/>
+      <c r="V5" s="46"/>
+      <c r="W5" s="46"/>
+      <c r="X5" s="46"/>
+      <c r="Y5" s="46"/>
+      <c r="Z5" s="46"/>
+      <c r="AA5" s="46"/>
+      <c r="AB5" s="47">
         <v>3</v>
       </c>
-      <c r="AC5" s="40"/>
-      <c r="AD5" s="40"/>
-      <c r="AE5" s="40"/>
+      <c r="AC5" s="47"/>
+      <c r="AD5" s="47"/>
+      <c r="AE5" s="47"/>
     </row>
     <row r="6" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q6" s="46">
+      <c r="Q6" s="43">
         <v>2</v>
       </c>
       <c r="R6" s="1" t="s">
@@ -1295,7 +1320,7 @@
       <c r="A7" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="Q7" s="46"/>
+      <c r="Q7" s="43"/>
       <c r="R7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1341,6 +1366,14 @@
       <c r="A8" s="24" t="s">
         <v>19</v>
       </c>
+      <c r="B8" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
@@ -1364,27 +1397,33 @@
       <c r="A9" s="24" t="s">
         <v>20</v>
       </c>
+      <c r="B9" s="51"/>
+      <c r="C9" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="S9" s="1"/>
-      <c r="T9" s="40">
+      <c r="T9" s="47">
         <v>3</v>
       </c>
-      <c r="U9" s="40"/>
-      <c r="V9" s="40"/>
-      <c r="W9" s="40"/>
-      <c r="X9" s="39">
+      <c r="U9" s="47"/>
+      <c r="V9" s="47"/>
+      <c r="W9" s="47"/>
+      <c r="X9" s="46">
         <v>2</v>
       </c>
-      <c r="Y9" s="39"/>
-      <c r="Z9" s="39"/>
-      <c r="AA9" s="39"/>
-      <c r="AB9" s="39"/>
-      <c r="AC9" s="39"/>
-      <c r="AD9" s="39"/>
-      <c r="AE9" s="39"/>
+      <c r="Y9" s="46"/>
+      <c r="Z9" s="46"/>
+      <c r="AA9" s="46"/>
+      <c r="AB9" s="46"/>
+      <c r="AC9" s="46"/>
+      <c r="AD9" s="46"/>
+      <c r="AE9" s="46"/>
       <c r="AG9" s="14"/>
       <c r="AH9" s="14"/>
     </row>
@@ -1392,8 +1431,14 @@
       <c r="A10" s="24" t="s">
         <v>21</v>
       </c>
+      <c r="B10" s="51"/>
+      <c r="C10" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
       <c r="P10" s="32"/>
-      <c r="Q10" s="46">
+      <c r="Q10" s="43">
         <v>3</v>
       </c>
       <c r="R10" s="1" t="s">
@@ -1433,7 +1478,13 @@
       <c r="A11" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="Q11" s="46"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="Q11" s="43"/>
       <c r="R11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1481,6 +1532,12 @@
       <c r="A12" s="24" t="s">
         <v>23</v>
       </c>
+      <c r="B12" s="51"/>
+      <c r="C12" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
@@ -1504,27 +1561,33 @@
       <c r="A13" s="24" t="s">
         <v>24</v>
       </c>
+      <c r="B13" s="51"/>
+      <c r="C13" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="S13" s="1"/>
-      <c r="T13" s="41">
+      <c r="T13" s="48">
         <v>1</v>
       </c>
-      <c r="U13" s="41"/>
-      <c r="V13" s="41"/>
-      <c r="W13" s="41"/>
-      <c r="X13" s="41"/>
-      <c r="Y13" s="41"/>
-      <c r="Z13" s="41"/>
-      <c r="AA13" s="41"/>
-      <c r="AB13" s="42">
+      <c r="U13" s="48"/>
+      <c r="V13" s="48"/>
+      <c r="W13" s="48"/>
+      <c r="X13" s="48"/>
+      <c r="Y13" s="48"/>
+      <c r="Z13" s="48"/>
+      <c r="AA13" s="48"/>
+      <c r="AB13" s="49">
         <v>0</v>
       </c>
-      <c r="AC13" s="42"/>
-      <c r="AD13" s="42"/>
-      <c r="AE13" s="42"/>
+      <c r="AC13" s="49"/>
+      <c r="AD13" s="49"/>
+      <c r="AE13" s="49"/>
       <c r="AG13" s="14"/>
       <c r="AH13" s="14"/>
     </row>
@@ -1532,7 +1595,13 @@
       <c r="A14" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="Q14" s="46">
+      <c r="B14" s="51"/>
+      <c r="C14" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="Q14" s="43">
         <v>4</v>
       </c>
       <c r="R14" s="1" t="s">
@@ -1572,7 +1641,7 @@
       <c r="A15" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="Q15" s="46"/>
+      <c r="Q15" s="43"/>
       <c r="R15" s="1" t="s">
         <v>5</v>
       </c>
@@ -1618,6 +1687,14 @@
       <c r="AH15" s="14"/>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A16" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
@@ -1642,25 +1719,25 @@
         <v>14</v>
       </c>
       <c r="S17" s="1"/>
-      <c r="T17" s="40">
+      <c r="T17" s="47">
         <v>0</v>
       </c>
-      <c r="U17" s="40"/>
-      <c r="V17" s="40"/>
-      <c r="W17" s="40"/>
-      <c r="X17" s="39">
+      <c r="U17" s="47"/>
+      <c r="V17" s="47"/>
+      <c r="W17" s="47"/>
+      <c r="X17" s="46">
         <v>7</v>
       </c>
-      <c r="Y17" s="39"/>
-      <c r="Z17" s="39"/>
-      <c r="AA17" s="39"/>
-      <c r="AB17" s="39"/>
-      <c r="AC17" s="39"/>
-      <c r="AD17" s="39"/>
-      <c r="AE17" s="39"/>
+      <c r="Y17" s="46"/>
+      <c r="Z17" s="46"/>
+      <c r="AA17" s="46"/>
+      <c r="AB17" s="46"/>
+      <c r="AC17" s="46"/>
+      <c r="AD17" s="46"/>
+      <c r="AE17" s="46"/>
     </row>
     <row r="18" spans="14:32" x14ac:dyDescent="0.25">
-      <c r="Q18" s="46">
+      <c r="Q18" s="43">
         <v>5</v>
       </c>
       <c r="R18" s="1" t="s">
@@ -1695,7 +1772,7 @@
       </c>
     </row>
     <row r="19" spans="14:32" x14ac:dyDescent="0.25">
-      <c r="Q19" s="46"/>
+      <c r="Q19" s="43"/>
       <c r="R19" s="1" t="s">
         <v>5</v>
       </c>
@@ -1777,7 +1854,7 @@
       <c r="AE21" s="1"/>
     </row>
     <row r="22" spans="14:32" x14ac:dyDescent="0.25">
-      <c r="Q22" s="46">
+      <c r="Q22" s="43">
         <v>6</v>
       </c>
       <c r="R22" s="1" t="s">
@@ -1800,7 +1877,7 @@
       <c r="AE22" s="1"/>
     </row>
     <row r="23" spans="14:32" x14ac:dyDescent="0.25">
-      <c r="Q23" s="46"/>
+      <c r="Q23" s="43"/>
       <c r="R23" s="1" t="s">
         <v>5</v>
       </c>
@@ -1949,7 +2026,25 @@
       <c r="AE31" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="31">
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="X17:AE17"/>
+    <mergeCell ref="AB5:AE5"/>
+    <mergeCell ref="T1:W1"/>
+    <mergeCell ref="X1:AE1"/>
+    <mergeCell ref="T5:AA5"/>
+    <mergeCell ref="T9:W9"/>
+    <mergeCell ref="X9:AE9"/>
+    <mergeCell ref="T13:AA13"/>
+    <mergeCell ref="AB13:AE13"/>
+    <mergeCell ref="T17:W17"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="N2:N3"/>
@@ -1962,16 +2057,7 @@
     <mergeCell ref="Q10:Q11"/>
     <mergeCell ref="Q14:Q15"/>
     <mergeCell ref="Q18:Q19"/>
-    <mergeCell ref="X17:AE17"/>
-    <mergeCell ref="AB5:AE5"/>
-    <mergeCell ref="T1:W1"/>
-    <mergeCell ref="X1:AE1"/>
-    <mergeCell ref="T5:AA5"/>
-    <mergeCell ref="T9:W9"/>
-    <mergeCell ref="X9:AE9"/>
-    <mergeCell ref="T13:AA13"/>
-    <mergeCell ref="AB13:AE13"/>
-    <mergeCell ref="T17:W17"/>
+    <mergeCell ref="B8:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>